<commit_message>
Added more data to the BOM
</commit_message>
<xml_diff>
--- a/eagle/T06_LockBox_bom.xlsx
+++ b/eagle/T06_LockBox_bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="0" windowWidth="25820" windowHeight="17560"/>
+    <workbookView xWindow="-60" yWindow="0" windowWidth="13480" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="T06_LockBox_Bom1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="244">
   <si>
     <t>Part</t>
   </si>
@@ -719,6 +719,39 @@
   </si>
   <si>
     <t>541-150CCT-ND</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>P4.7KACT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-6GEYJ472V</t>
+  </si>
+  <si>
+    <t>PNHD</t>
+  </si>
+  <si>
+    <t>1X10</t>
+  </si>
+  <si>
+    <t>10POS SIL VERTICAL PIN HEADER</t>
+  </si>
+  <si>
+    <t>Harwin Inc</t>
+  </si>
+  <si>
+    <t>M20-9991046</t>
+  </si>
+  <si>
+    <t>952-1843-ND</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1211,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="144">
+  <cellStyleXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1323,15 +1356,71 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1341,8 +1430,14 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="144">
+  <cellStyles count="206">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1422,6 +1517,37 @@
     <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1478,6 +1604,37 @@
     <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1778,1072 +1935,1390 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6400" topLeftCell="C1" activePane="topRight"/>
-      <selection activeCell="J22" sqref="J22"/>
-      <selection pane="topRight" activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane xSplit="6400" activePane="topRight"/>
+      <selection activeCell="H21" sqref="H21:M21"/>
+      <selection pane="topRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3"/>
-    <col min="2" max="2" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="37.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" style="3" customWidth="1"/>
-    <col min="11" max="12" width="8.83203125" style="3"/>
-    <col min="13" max="13" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="1" customWidth="1"/>
+    <col min="11" max="12" width="8.83203125" style="1"/>
+    <col min="13" max="13" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="1">
         <v>1</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="1">
         <v>10</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="1">
         <v>100</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="1">
         <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="3">
         <v>0.26</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="3">
         <v>2.1800000000000002</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="3">
         <v>10.88</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="3">
         <v>63.92</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="3">
         <v>0.34</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="3">
         <v>2.8</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="3">
         <v>14</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="3">
         <v>82.25</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="3">
         <v>0.12</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="3">
         <v>0.87</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="3">
         <v>3.97</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="3">
         <v>21.66</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="1" t="s">
         <v>171</v>
       </c>
       <c r="J6" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="K6" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="L6" s="3">
+        <v>14</v>
+      </c>
+      <c r="M6" s="3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="L7" s="3">
+        <v>3.34</v>
+      </c>
+      <c r="M7" s="3">
+        <v>18.21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="L8" s="3">
+        <v>3.34</v>
+      </c>
+      <c r="M8" s="3">
+        <v>18.21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="L9" s="3">
+        <v>3.34</v>
+      </c>
+      <c r="M9" s="3">
+        <v>18.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="L10" s="3">
+        <v>7.88</v>
+      </c>
+      <c r="M10" s="3">
+        <v>26.27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="3">
-        <v>0.1336</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="F12" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="K12" s="3">
+        <v>3.77</v>
+      </c>
+      <c r="L12" s="3">
+        <v>26.36</v>
+      </c>
+      <c r="M12" s="3">
+        <v>188.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="K13" s="3">
+        <v>3.07</v>
+      </c>
+      <c r="L13" s="3">
+        <v>21.51</v>
+      </c>
+      <c r="M13" s="3">
+        <v>153.65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="K14" s="3">
+        <v>2.48</v>
+      </c>
+      <c r="L14" s="3">
+        <v>17.16</v>
+      </c>
+      <c r="M14" s="3">
+        <v>118.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="M15" s="3">
+        <v>20.36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="M16" s="3">
+        <v>20.36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="M17" s="3">
+        <v>20.36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="L18" s="3">
+        <v>2.19</v>
+      </c>
+      <c r="M18" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="1">
+        <v>150</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="M19" s="3">
+        <v>20.36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="1">
+        <v>33</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="M20" s="3">
+        <v>20.36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="1">
+        <v>33</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="M21" s="3">
+        <v>20.36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="M22" s="3">
+        <v>20.36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="L23" s="3">
+        <v>1.49</v>
+      </c>
+      <c r="M23" s="3">
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="L24" s="3">
+        <v>1.49</v>
+      </c>
+      <c r="M24" s="3">
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="M25" s="3">
+        <v>20.36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="K27" s="3">
+        <v>1.73</v>
+      </c>
+      <c r="L27" s="3">
+        <v>11.34</v>
+      </c>
+      <c r="M27" s="3">
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="K28" s="3">
+        <v>1.73</v>
+      </c>
+      <c r="L28" s="3">
+        <v>11.34</v>
+      </c>
+      <c r="M28" s="3">
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="K29" s="3">
+        <v>1.73</v>
+      </c>
+      <c r="L29" s="3">
+        <v>11.34</v>
+      </c>
+      <c r="M29" s="3">
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J30" s="3">
+        <v>3.74</v>
+      </c>
+      <c r="K30" s="3">
+        <v>33.380000000000003</v>
+      </c>
+      <c r="L30" s="3">
+        <v>273.74</v>
+      </c>
+      <c r="M30" s="3">
+        <v>1869.45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J31" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="K31" s="1">
+        <v>8.92</v>
+      </c>
+      <c r="L31" s="1">
+        <v>68.67</v>
+      </c>
+      <c r="M31" s="1">
+        <v>407.55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J32" s="1">
+        <v>1</v>
+      </c>
+      <c r="K32" s="1">
         <v>7</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="J7" s="3">
-        <v>25</v>
-      </c>
-      <c r="K7" s="3">
-        <v>5.96E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0.13</v>
-      </c>
-      <c r="K10" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="L10" s="5">
-        <v>7.88</v>
-      </c>
-      <c r="M10" s="5">
-        <v>26.27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="J15" s="3">
-        <v>50</v>
-      </c>
-      <c r="K15" s="3">
-        <v>4.82E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="J18" s="3">
-        <v>10</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="3">
-        <v>150</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="3">
-        <v>33</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="3">
-        <v>27</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="3" t="s">
+      <c r="L32" s="1">
         <v>47</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="3" t="s">
+      <c r="M32" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="J27" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="K27" s="5">
-        <v>1.73</v>
-      </c>
-      <c r="L27" s="5">
-        <v>11.34</v>
-      </c>
-      <c r="M27" s="5">
-        <v>37.799999999999997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="J28" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="K28" s="5">
-        <v>1.73</v>
-      </c>
-      <c r="L28" s="5">
-        <v>11.34</v>
-      </c>
-      <c r="M28" s="5">
-        <v>37.799999999999997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="J29" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="K29" s="5">
-        <v>1.73</v>
-      </c>
-      <c r="L29" s="5">
-        <v>11.34</v>
-      </c>
-      <c r="M29" s="5">
-        <v>37.799999999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="J30" s="5">
-        <v>3.74</v>
-      </c>
-      <c r="K30" s="5">
-        <v>33.380000000000003</v>
-      </c>
-      <c r="L30" s="5">
-        <v>273.74</v>
-      </c>
-      <c r="M30" s="5">
-        <v>1869.45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J31" s="3">
-        <v>1.02</v>
-      </c>
-      <c r="K31" s="3">
-        <v>8.92</v>
-      </c>
-      <c r="L31" s="3">
-        <v>68.67</v>
-      </c>
-      <c r="M31" s="3">
-        <v>407.55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="J32" s="3">
-        <v>1</v>
-      </c>
-      <c r="K32" s="3">
-        <v>7</v>
-      </c>
-      <c r="L32" s="3">
-        <v>47</v>
-      </c>
-      <c r="M32" s="3">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      <c r="H33" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="I33" s="3" t="s">
+      <c r="I33" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="J33" s="5">
+      <c r="J33" s="3">
         <v>0.96</v>
       </c>
-      <c r="K33" s="5">
+      <c r="K33" s="3">
         <v>8.52</v>
       </c>
-      <c r="L33" s="5">
+      <c r="L33" s="3">
         <v>67.349999999999994</v>
       </c>
-      <c r="M33" s="5">
+      <c r="M33" s="3">
         <v>412.35</v>
       </c>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="I34" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="J34" s="5">
+      <c r="J34" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="K34" s="5">
+      <c r="K34" s="3">
         <v>5.35</v>
       </c>
-      <c r="L34" s="5">
+      <c r="L34" s="3">
         <v>41.01</v>
       </c>
-      <c r="M34" s="5">
+      <c r="M34" s="3">
         <v>294.2</v>
       </c>
     </row>
     <row r="35" spans="1:13">
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="1" t="s">
         <v>213</v>
       </c>
       <c r="I35" t="s">
         <v>214</v>
       </c>
-      <c r="J35" s="5">
+      <c r="J35" s="3">
         <v>0.49</v>
       </c>
-      <c r="K35" s="5">
+      <c r="K35" s="3">
         <v>3.83</v>
       </c>
-      <c r="L35" s="5">
+      <c r="L35" s="3">
         <v>26.35</v>
       </c>
-      <c r="M35" s="5">
+      <c r="M35" s="3">
         <v>135.05000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="B36" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I36" t="s">
+        <v>243</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="K36" s="3">
+        <v>3.33</v>
+      </c>
+      <c r="L36" s="3">
+        <v>23.28</v>
+      </c>
+      <c r="M36" s="3">
+        <v>166.25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J1:M1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:D2"/>
@@ -2853,7 +3328,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="J1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Added cost for main and lcd pcb
</commit_message>
<xml_diff>
--- a/eagle/T06_LockBox_bom.xlsx
+++ b/eagle/T06_LockBox_bom.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="0" windowWidth="13480" windowHeight="17560"/>
+    <workbookView xWindow="5820" yWindow="0" windowWidth="22900" windowHeight="17560"/>
+    <workbookView minimized="1" xWindow="3520" yWindow="3320" windowWidth="25380" windowHeight="17560" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="T06_LockBox_Bom1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Main_Board" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="181">
   <si>
     <t>Part</t>
   </si>
@@ -238,273 +239,6 @@
     <t>8-Pin eithernet jack</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Index Quantity Part Number Manufacturer Part</t>
-  </si>
-  <si>
-    <t>Number Description Customer</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>Backorder</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Extended</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 5 CP-102A-ND PJ-102A</t>
-  </si>
-  <si>
-    <t>CONN</t>
-  </si>
-  <si>
-    <t>JACK</t>
-  </si>
-  <si>
-    <t>POWER</t>
-  </si>
-  <si>
-    <t>2.1MM PCB</t>
-  </si>
-  <si>
-    <t>Immediate 0 1.00000 $5.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2 6 609-3210-ND 67996-206HLF</t>
-  </si>
-  <si>
-    <t>HEADER</t>
-  </si>
-  <si>
-    <t>6POS .100</t>
-  </si>
-  <si>
-    <t>STR 15AU</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.40000 $2.40</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3 3 609-3391-ND 67996-408HLF</t>
-  </si>
-  <si>
-    <t>8POS .100</t>
-  </si>
-  <si>
-    <t>STR TIN</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.32000 $0.96</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4 25 2N3904FS-ND 2N3904BU</t>
-  </si>
-  <si>
-    <t>IC TRANS</t>
-  </si>
-  <si>
-    <t>NPN SS GP</t>
-  </si>
-  <si>
-    <t>200MA</t>
-  </si>
-  <si>
-    <t>TO-92</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.15760 $3.94</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5 2 609-1046-ND 54602-908LF</t>
-  </si>
-  <si>
-    <t>MOD JACK</t>
-  </si>
-  <si>
-    <t>R/A 8P8C</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.57000 $1.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6 5 609-3243-ND 67997-410HLF</t>
-  </si>
-  <si>
-    <t>10POS .100</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.26000 $1.30</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7 10 1276-1066-1-ND CL21B105KAFNNNE</t>
-  </si>
-  <si>
-    <t>CAP CER</t>
-  </si>
-  <si>
-    <t>1UF 25V</t>
-  </si>
-  <si>
-    <t>10% X7R</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.07100 $0.71</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8 10 1276-1804-1-ND CL31B106KAHNNNE</t>
-  </si>
-  <si>
-    <t>10UF 25V</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.19800 $1.98</t>
-  </si>
-  <si>
-    <t>Digi-Key - Online Order Summary https://www.digikey.com/classic/Ordering/PrintView.aspx?CS...</t>
-  </si>
-  <si>
-    <t>1 of 2 11/3/14 7:58 PM 9 10 490-1677-1-ND GRM21BR71E334KA01L</t>
-  </si>
-  <si>
-    <t>0.33UF 25V</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.21800 $2.18</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10 25 1276-1275-1-ND CL21B105KPFNNNE</t>
-  </si>
-  <si>
-    <t>1UF 10V</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.05960 $1.49</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11 25 1276-2934-1-ND CL21B106KPQNFNE</t>
-  </si>
-  <si>
-    <t>10UF 10V</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.13360 $3.34</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 12 10 P1.00KCCT-ND ERJ-6ENF1001V</t>
-  </si>
-  <si>
-    <t>RES 1K</t>
-  </si>
-  <si>
-    <t>OHM 1/8W</t>
-  </si>
-  <si>
-    <t>1% 0805</t>
-  </si>
-  <si>
-    <t>SMD</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.10000 $1.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 13 20 541-33.0CCT-ND CRCW080533R0FKEA</t>
-  </si>
-  <si>
-    <t>RES 33.0</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.08900 $1.78</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 14 10 541-150CCT-ND CRCW0805150RFKEA</t>
-  </si>
-  <si>
-    <t>RES 150</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.08900 $0.89</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 15 50 541-10.0KCCT-ND CRCW080510K0FKEA</t>
-  </si>
-  <si>
-    <t>RES 10.0K</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.04820 $2.41</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 16 1 S6105-ND PPTC052LFBN-RC</t>
-  </si>
-  <si>
-    <t>FEM</t>
-  </si>
-  <si>
-    <t>10POS .1"</t>
-  </si>
-  <si>
-    <t>DL TIN</t>
-  </si>
-  <si>
-    <t>Immediate 0 0.85000 $0.85</t>
-  </si>
-  <si>
-    <t>Subtotal $31.37</t>
-  </si>
-  <si>
-    <t>Shipping Estimate</t>
-  </si>
-  <si>
-    <t>Sales Tax $0.00</t>
-  </si>
-  <si>
-    <t>Total unknown</t>
-  </si>
-  <si>
-    <t>Fields marked as unknown cannot be determined at this time.</t>
-  </si>
-  <si>
-    <t>Applicable taxes will be added to your order at submit time unless you have a tax exempt certificate on file with us.</t>
-  </si>
-  <si>
-    <t>All duties and taxes are the responsibility of the customer.</t>
-  </si>
-  <si>
-    <t>These commodities, technology or software will be exported from the United States in accordance with the Export Administration</t>
-  </si>
-  <si>
-    <t>regulation. Diversion contrary to U.S. law prohibited.</t>
-  </si>
-  <si>
-    <t>Note: If your package is of excessive weight and size, someone will contact you prior to shipping and notify you of shipping costs.</t>
-  </si>
-  <si>
-    <t>Shipping charges will be prepaid and added to your order.</t>
-  </si>
-  <si>
-    <t>Order Notes:</t>
-  </si>
-  <si>
-    <t>COMMIT LANGUAGE: ENGLISH</t>
-  </si>
-  <si>
-    <t>2 of 2 1</t>
-  </si>
-  <si>
     <t>Manufacturer Part Number</t>
   </si>
   <si>
@@ -752,6 +486,84 @@
   </si>
   <si>
     <t>952-1843-ND</t>
+  </si>
+  <si>
+    <t>IC-SOCKET</t>
+  </si>
+  <si>
+    <t>IC SOCKET - 28POS</t>
+  </si>
+  <si>
+    <t>AE10286-ND</t>
+  </si>
+  <si>
+    <t>A28-LC-7-TT-R</t>
+  </si>
+  <si>
+    <t>Assmann WSW Components</t>
+  </si>
+  <si>
+    <t>Lock-style Solenoid 12VDC</t>
+  </si>
+  <si>
+    <t>ADAFRUIT</t>
+  </si>
+  <si>
+    <t>12V / 500mA</t>
+  </si>
+  <si>
+    <t>SOLENOID</t>
+  </si>
+  <si>
+    <t>NES CONTROLLER</t>
+  </si>
+  <si>
+    <t>Original Nintendo Controler</t>
+  </si>
+  <si>
+    <t>Nintendo</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>4.7K</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>PART</t>
+  </si>
+  <si>
+    <t>LCD Display - RGB LED Backlit</t>
+  </si>
+  <si>
+    <t>Newhaven Display Intl</t>
+  </si>
+  <si>
+    <t>NHD-C0220BIZ-FS(RGB)-FBW-3VM-ND</t>
+  </si>
+  <si>
+    <t>NHD-C0220BIZ-FS(RGB)-FBW-3VM</t>
+  </si>
+  <si>
+    <t>PCB - Main</t>
+  </si>
+  <si>
+    <t>PCB - LockBox Main board</t>
+  </si>
+  <si>
+    <t>OSHPark</t>
+  </si>
+  <si>
+    <t>PCB - LCD screen</t>
+  </si>
+  <si>
+    <t>PCB - LCD</t>
   </si>
 </sst>
 </file>
@@ -759,7 +571,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1095,7 +907,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1210,8 +1022,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="206">
+  <cellStyleXfs count="242">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1418,8 +1310,44 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1427,17 +1355,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="206">
+  <cellStyles count="242">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1548,6 +1530,24 @@
     <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1635,6 +1635,24 @@
     <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1935,90 +1953,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane xSplit="6400" activePane="topRight"/>
-      <selection activeCell="H21" sqref="H21:M21"/>
-      <selection pane="topRight" activeCell="E27" sqref="E27"/>
+      <pane xSplit="6900" activePane="topRight"/>
+      <selection activeCell="G42" sqref="G42"/>
+      <selection pane="topRight" activeCell="K42" sqref="K42"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="37.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" style="1" customWidth="1"/>
-    <col min="11" max="12" width="8.83203125" style="1"/>
-    <col min="13" max="13" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="1"/>
+    <col min="10" max="10" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" style="1" customWidth="1"/>
+    <col min="12" max="13" width="8.83203125" style="1"/>
+    <col min="14" max="14" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14" customHeight="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:14" ht="14" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="1">
+      <c r="K1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10">
         <v>1</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="10">
         <v>10</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="10">
         <v>100</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="11">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2032,34 +2058,34 @@
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>163</v>
+        <v>74</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>184</v>
+        <v>95</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>207</v>
+        <v>118</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J3" s="3">
+        <v>80</v>
+      </c>
+      <c r="K3" s="23">
         <v>0.26</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="23">
         <v>2.1800000000000002</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="23">
         <v>10.88</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="23">
         <v>63.92</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2073,34 +2099,34 @@
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>163</v>
+        <v>74</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>184</v>
+        <v>95</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>208</v>
+        <v>119</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>164</v>
+        <v>75</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="J4" s="3">
+        <v>76</v>
+      </c>
+      <c r="K4" s="23">
         <v>0.34</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="23">
         <v>2.8</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="23">
         <v>14</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="23">
         <v>82.25</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -2114,34 +2140,34 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>163</v>
+        <v>74</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>184</v>
+        <v>95</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>208</v>
+        <v>119</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>166</v>
+        <v>77</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="J5" s="3">
+        <v>78</v>
+      </c>
+      <c r="K5" s="23">
         <v>0.12</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="23">
         <v>0.87</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="23">
         <v>3.97</v>
       </c>
-      <c r="M5" s="3">
+      <c r="N5" s="23">
         <v>21.66</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -2155,34 +2181,34 @@
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>184</v>
+        <v>95</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>208</v>
+        <v>119</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>170</v>
+        <v>81</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="J6" s="3">
+        <v>82</v>
+      </c>
+      <c r="K6" s="23">
         <v>0.32</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="23">
         <v>2.8</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="23">
         <v>14</v>
       </c>
-      <c r="M6" s="3">
+      <c r="N6" s="23">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -2196,34 +2222,34 @@
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>184</v>
+        <v>95</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>208</v>
+        <v>119</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="J7" s="3">
+        <v>84</v>
+      </c>
+      <c r="K7" s="23">
         <v>0.1</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="23">
         <v>0.73</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="23">
         <v>3.34</v>
       </c>
-      <c r="M7" s="3">
+      <c r="N7" s="23">
         <v>18.21</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2237,34 +2263,34 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>184</v>
+        <v>95</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>208</v>
+        <v>119</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="J8" s="3">
+        <v>84</v>
+      </c>
+      <c r="K8" s="23">
         <v>0.1</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="23">
         <v>0.73</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="23">
         <v>3.34</v>
       </c>
-      <c r="M8" s="3">
+      <c r="N8" s="23">
         <v>18.21</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -2278,34 +2304,34 @@
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>184</v>
+        <v>95</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>208</v>
+        <v>119</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="J9" s="3">
+        <v>84</v>
+      </c>
+      <c r="K9" s="23">
         <v>0.1</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="23">
         <v>0.73</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="23">
         <v>3.34</v>
       </c>
-      <c r="M9" s="3">
+      <c r="N9" s="23">
         <v>18.21</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -2319,39 +2345,39 @@
         <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>203</v>
+        <v>114</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>204</v>
+        <v>115</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>202</v>
+        <v>113</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>205</v>
+        <v>116</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="J10" s="3">
+        <v>112</v>
+      </c>
+      <c r="K10" s="23">
         <v>0.13</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L10" s="23">
         <v>1.2</v>
       </c>
-      <c r="L10" s="3">
+      <c r="M10" s="23">
         <v>7.88</v>
       </c>
-      <c r="M10" s="3">
+      <c r="N10" s="23">
         <v>26.27</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>178</v>
+        <v>89</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
@@ -2360,15 +2386,19 @@
         <v>22</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>98</v>
+      </c>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>178</v>
+        <v>89</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>26</v>
@@ -2377,36 +2407,36 @@
         <v>25</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>186</v>
+        <v>97</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>218</v>
+        <v>129</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>193</v>
+        <v>104</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="J12" s="3">
+        <v>105</v>
+      </c>
+      <c r="K12" s="23">
         <v>0.4</v>
       </c>
-      <c r="K12" s="3">
+      <c r="L12" s="23">
         <v>3.77</v>
       </c>
-      <c r="L12" s="3">
+      <c r="M12" s="23">
         <v>26.36</v>
       </c>
-      <c r="M12" s="3">
+      <c r="N12" s="23">
         <v>188.3</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>178</v>
+        <v>89</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>29</v>
@@ -2415,36 +2445,36 @@
         <v>28</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>188</v>
+        <v>99</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>218</v>
+        <v>129</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>196</v>
+        <v>107</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="J13" s="3">
+        <v>106</v>
+      </c>
+      <c r="K13" s="23">
         <v>0.32</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L13" s="23">
         <v>3.07</v>
       </c>
-      <c r="L13" s="3">
+      <c r="M13" s="23">
         <v>21.51</v>
       </c>
-      <c r="M13" s="3">
+      <c r="N13" s="23">
         <v>153.65</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>178</v>
+        <v>89</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -2453,36 +2483,36 @@
         <v>31</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>189</v>
+        <v>100</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>218</v>
+        <v>129</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>199</v>
+        <v>110</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="J14" s="3">
+        <v>111</v>
+      </c>
+      <c r="K14" s="23">
         <v>0.26</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="23">
         <v>2.48</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14" s="23">
         <v>17.16</v>
       </c>
-      <c r="M14" s="3">
+      <c r="N14" s="23">
         <v>118.8</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>35</v>
@@ -2491,39 +2521,39 @@
         <v>34</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>233</v>
+        <v>144</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>174</v>
+        <v>85</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="K15" s="3">
+        <v>86</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="L15" s="23">
         <v>0.97</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="M15" s="3">
+      <c r="M15" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="N15" s="23">
         <v>20.36</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>35</v>
@@ -2532,39 +2562,39 @@
         <v>34</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>233</v>
+        <v>144</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>174</v>
+        <v>85</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="K16" s="3">
+        <v>86</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="L16" s="23">
         <v>0.97</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="M16" s="3">
+      <c r="M16" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="N16" s="23">
         <v>20.36</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>35</v>
@@ -2573,39 +2603,39 @@
         <v>34</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>233</v>
+        <v>144</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>174</v>
+        <v>85</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="K17" s="3">
+        <v>86</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="L17" s="23">
         <v>0.97</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="M17" s="3">
+      <c r="M17" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="N17" s="23">
         <v>20.36</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>35</v>
@@ -2614,39 +2644,39 @@
         <v>39</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>235</v>
+        <v>146</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>176</v>
+        <v>87</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="J18" s="3">
+        <v>88</v>
+      </c>
+      <c r="K18" s="23">
         <v>0.1</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="L18" s="3">
+      <c r="L18" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="M18" s="23">
         <v>2.19</v>
       </c>
-      <c r="M18" s="3">
+      <c r="N18" s="23">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>35</v>
@@ -2655,39 +2685,39 @@
         <v>150</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>233</v>
+        <v>144</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>231</v>
+        <v>142</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="K19" s="3">
+        <v>143</v>
+      </c>
+      <c r="K19" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="L19" s="23">
         <v>0.97</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="M19" s="3">
+      <c r="M19" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="N19" s="23">
         <v>20.36</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>35</v>
@@ -2696,39 +2726,39 @@
         <v>33</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>233</v>
+        <v>144</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>228</v>
+        <v>139</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="K20" s="3">
+        <v>140</v>
+      </c>
+      <c r="K20" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="L20" s="23">
         <v>0.97</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="M20" s="3">
+      <c r="M20" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="N20" s="23">
         <v>20.36</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>35</v>
@@ -2737,39 +2767,39 @@
         <v>33</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>233</v>
+        <v>144</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>228</v>
+        <v>139</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="K21" s="3">
+        <v>140</v>
+      </c>
+      <c r="K21" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="L21" s="23">
         <v>0.97</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="M21" s="3">
+      <c r="M21" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="N21" s="23">
         <v>20.36</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>35</v>
@@ -2778,39 +2808,39 @@
         <v>34</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>233</v>
+        <v>144</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>174</v>
+        <v>85</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="K22" s="3">
+        <v>86</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="L22" s="23">
         <v>0.97</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="M22" s="3">
+      <c r="M22" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="N22" s="23">
         <v>20.36</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>35</v>
@@ -2819,39 +2849,39 @@
         <v>45</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>235</v>
+        <v>146</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>237</v>
+        <v>148</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="J23" s="3">
+        <v>147</v>
+      </c>
+      <c r="K23" s="23">
         <v>0.1</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="L23" s="3">
+      <c r="L23" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="M23" s="23">
         <v>1.49</v>
       </c>
-      <c r="M23" s="3">
+      <c r="N23" s="23">
         <v>5.44</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>35</v>
@@ -2860,39 +2890,39 @@
         <v>45</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>235</v>
+        <v>146</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>237</v>
+        <v>148</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="J24" s="3">
+        <v>147</v>
+      </c>
+      <c r="K24" s="23">
         <v>0.1</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="L24" s="3">
+      <c r="L24" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="M24" s="23">
         <v>1.49</v>
       </c>
-      <c r="M24" s="3">
+      <c r="N24" s="23">
         <v>5.44</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>35</v>
@@ -2901,51 +2931,55 @@
         <v>34</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>233</v>
+        <v>144</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>174</v>
+        <v>85</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="K25" s="3">
+        <v>86</v>
+      </c>
+      <c r="K25" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="L25" s="23">
         <v>0.97</v>
       </c>
-      <c r="L25" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="M25" s="3">
+      <c r="M25" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="N25" s="23">
         <v>20.36</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>190</v>
+        <v>101</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+        <v>91</v>
+      </c>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -2965,25 +2999,25 @@
         <v>68</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>197</v>
+        <v>108</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="J27" s="3">
+        <v>109</v>
+      </c>
+      <c r="K27" s="23">
         <v>0.19</v>
       </c>
-      <c r="K27" s="3">
+      <c r="L27" s="23">
         <v>1.73</v>
       </c>
-      <c r="L27" s="3">
+      <c r="M27" s="23">
         <v>11.34</v>
       </c>
-      <c r="M27" s="3">
+      <c r="N27" s="23">
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
@@ -3003,25 +3037,25 @@
         <v>68</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>197</v>
+        <v>108</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="J28" s="3">
+        <v>109</v>
+      </c>
+      <c r="K28" s="23">
         <v>0.19</v>
       </c>
-      <c r="K28" s="3">
+      <c r="L28" s="23">
         <v>1.73</v>
       </c>
-      <c r="L28" s="3">
+      <c r="M28" s="23">
         <v>11.34</v>
       </c>
-      <c r="M28" s="3">
+      <c r="N28" s="23">
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
         <v>54</v>
       </c>
@@ -3041,25 +3075,25 @@
         <v>68</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>197</v>
+        <v>108</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="J29" s="3">
+        <v>109</v>
+      </c>
+      <c r="K29" s="23">
         <v>0.19</v>
       </c>
-      <c r="K29" s="3">
+      <c r="L29" s="23">
         <v>1.73</v>
       </c>
-      <c r="L29" s="3">
+      <c r="M29" s="23">
         <v>11.34</v>
       </c>
-      <c r="M29" s="3">
+      <c r="N29" s="23">
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
@@ -3076,28 +3110,28 @@
         <v>58</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>227</v>
+        <v>138</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>215</v>
+        <v>126</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="J30" s="3">
+        <v>137</v>
+      </c>
+      <c r="K30" s="23">
         <v>3.74</v>
       </c>
-      <c r="K30" s="3">
+      <c r="L30" s="23">
         <v>33.380000000000003</v>
       </c>
-      <c r="L30" s="3">
+      <c r="M30" s="23">
         <v>273.74</v>
       </c>
-      <c r="M30" s="3">
+      <c r="N30" s="23">
         <v>1869.45</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -3114,28 +3148,28 @@
         <v>62</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>219</v>
+        <v>130</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>220</v>
+        <v>131</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="1">
+      <c r="K31" s="23">
         <v>1.02</v>
       </c>
-      <c r="K31" s="1">
+      <c r="L31" s="23">
         <v>8.92</v>
       </c>
-      <c r="L31" s="1">
+      <c r="M31" s="23">
         <v>68.67</v>
       </c>
-      <c r="M31" s="1">
+      <c r="N31" s="23">
         <v>407.55</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>64</v>
       </c>
@@ -3149,69 +3183,69 @@
         <v>65</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>222</v>
+        <v>133</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>191</v>
+        <v>102</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>192</v>
+        <v>103</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="J32" s="1">
+        <v>132</v>
+      </c>
+      <c r="K32" s="23">
         <v>1</v>
       </c>
-      <c r="K32" s="1">
+      <c r="L32" s="23">
         <v>7</v>
       </c>
-      <c r="L32" s="1">
+      <c r="M32" s="23">
         <v>47</v>
       </c>
-      <c r="M32" s="1">
+      <c r="N32" s="23">
         <v>340</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>223</v>
+        <v>134</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>223</v>
+        <v>134</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>224</v>
+        <v>135</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>68</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>223</v>
+        <v>134</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="J33" s="3">
+        <v>136</v>
+      </c>
+      <c r="K33" s="23">
         <v>0.96</v>
       </c>
-      <c r="K33" s="3">
+      <c r="L33" s="23">
         <v>8.52</v>
       </c>
-      <c r="L33" s="3">
+      <c r="M33" s="23">
         <v>67.349999999999994</v>
       </c>
-      <c r="M33" s="3">
+      <c r="N33" s="23">
         <v>412.35</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>69</v>
       </c>
@@ -3219,7 +3253,7 @@
         <v>70</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>181</v>
+        <v>92</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>70</v>
@@ -3228,97 +3262,262 @@
         <v>71</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>218</v>
+        <v>129</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>216</v>
+        <v>127</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="J34" s="3">
+        <v>128</v>
+      </c>
+      <c r="K34" s="23">
         <v>0.56999999999999995</v>
       </c>
-      <c r="K34" s="3">
+      <c r="L34" s="23">
         <v>5.35</v>
       </c>
-      <c r="L34" s="3">
+      <c r="M34" s="23">
         <v>41.01</v>
       </c>
-      <c r="M34" s="3">
+      <c r="N34" s="23">
         <v>294.2</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:14">
       <c r="B35" s="1" t="s">
-        <v>209</v>
+        <v>120</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>210</v>
+        <v>121</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>209</v>
+        <v>120</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>211</v>
+        <v>122</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>212</v>
+        <v>123</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>213</v>
+        <v>124</v>
       </c>
       <c r="I35" t="s">
-        <v>214</v>
-      </c>
-      <c r="J35" s="3">
+        <v>125</v>
+      </c>
+      <c r="J35"/>
+      <c r="K35" s="23">
         <v>0.49</v>
       </c>
-      <c r="K35" s="3">
+      <c r="L35" s="23">
         <v>3.83</v>
       </c>
-      <c r="L35" s="3">
+      <c r="M35" s="23">
         <v>26.35</v>
       </c>
-      <c r="M35" s="3">
+      <c r="N35" s="23">
         <v>135.05000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:14">
       <c r="B36" s="1" t="s">
-        <v>238</v>
+        <v>149</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>239</v>
+        <v>150</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>240</v>
+        <v>151</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>241</v>
+        <v>152</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>242</v>
+        <v>153</v>
       </c>
       <c r="I36" t="s">
-        <v>243</v>
-      </c>
-      <c r="J36" s="3">
+        <v>154</v>
+      </c>
+      <c r="J36"/>
+      <c r="K36" s="23">
         <v>0.35</v>
       </c>
-      <c r="K36" s="3">
+      <c r="L36" s="23">
         <v>3.33</v>
       </c>
-      <c r="L36" s="3">
+      <c r="M36" s="23">
         <v>23.28</v>
       </c>
-      <c r="M36" s="3">
+      <c r="N36" s="23">
         <v>166.25</v>
       </c>
     </row>
+    <row r="37" spans="1:14">
+      <c r="B37" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K37" s="23">
+        <v>0.43</v>
+      </c>
+      <c r="L37" s="23">
+        <v>3.99</v>
+      </c>
+      <c r="M37" s="23">
+        <v>30.59</v>
+      </c>
+      <c r="N37" s="23">
+        <v>219.45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="B38" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1512</v>
+      </c>
+      <c r="K38" s="23">
+        <v>14.95</v>
+      </c>
+      <c r="L38" s="23">
+        <v>13.46</v>
+      </c>
+      <c r="M38" s="23">
+        <v>11.96</v>
+      </c>
+      <c r="N38" s="23"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="B39" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K39" s="23">
+        <v>7</v>
+      </c>
+      <c r="L39" s="23"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="B40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I40" t="s">
+        <v>174</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K40" s="23">
+        <v>12</v>
+      </c>
+      <c r="L40" s="23">
+        <v>105.6</v>
+      </c>
+      <c r="M40" s="23">
+        <v>948</v>
+      </c>
+      <c r="N40" s="23">
+        <f>2*4437.5</f>
+        <v>8875</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="B41" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K41" s="1">
+        <f>38.3/3</f>
+        <v>12.766666666666666</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="B42" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K42" s="1">
+        <f>26.6/3</f>
+        <v>8.8666666666666671</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="J1:M1"/>
+  <mergeCells count="11">
+    <mergeCell ref="K1:N1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:D2"/>
@@ -3328,11 +3527,13 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="G1:G2"/>
+    <mergeCell ref="J1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -3341,716 +3542,347 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A139"/>
+  <dimension ref="B1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection sqref="A1:A139"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="H2" sqref="H2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="53.1640625" customWidth="1"/>
+    <col min="3" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="2:11" ht="15" thickBot="1"/>
+    <row r="2" spans="2:11">
+      <c r="B2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="15" thickBot="1">
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="22"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="22"/>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16" t="str">
+        <f>T06_LockBox_Bom1!B30</f>
+        <v>ATMEGA328</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" s="18">
+        <v>1</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="18">
+        <v>1</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="18">
+        <v>3</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
+    <row r="9" spans="2:11">
+      <c r="B9" s="18">
+        <v>1</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
+      <c r="D9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" s="18">
+        <v>1</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" s="18">
+        <v>1</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12" s="18">
+        <v>1</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13" s="18">
+        <v>4</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31">
+      <c r="D13" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14" s="18">
+        <v>2</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="B15" s="18">
+        <v>1</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16" s="18">
+        <v>1</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="19">
+        <v>150</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="18">
+        <v>1</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="19">
+        <v>33</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
+      <c r="C18" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="18">
+        <v>1</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="18">
+        <v>1</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="18">
+        <v>1</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1">
-      <c r="A107" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1">
-      <c r="A109" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1">
-      <c r="A110" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1">
-      <c r="A112" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1">
-      <c r="A113" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
-      <c r="A116" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1">
-      <c r="A117" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1">
-      <c r="A118" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1">
-      <c r="A119" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1">
-      <c r="A120" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1">
-      <c r="A121" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1">
-      <c r="A122" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1">
-      <c r="A123">
+      <c r="D21" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:1">
-      <c r="A124" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1">
-      <c r="A125" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1">
-      <c r="A126" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1">
-      <c r="A127" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1">
-      <c r="A128" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1">
-      <c r="A129" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1">
-      <c r="A130" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1">
-      <c r="A131" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1">
-      <c r="A132" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1">
-      <c r="A133" t="s">
+      <c r="C22" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="2:5" ht="15" thickBot="1">
+      <c r="B23" s="12">
+        <v>1</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="134" spans="1:1">
-      <c r="A134" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1">
-      <c r="A135" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1">
-      <c r="A136" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1">
-      <c r="A137" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1">
-      <c r="A138" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1">
-      <c r="A139" t="s">
-        <v>160</v>
-      </c>
+      <c r="D23" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E23" s="14"/>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="D2:D3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
more changes to the bom
</commit_message>
<xml_diff>
--- a/eagle/T06_LockBox_bom.xlsx
+++ b/eagle/T06_LockBox_bom.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="0" windowWidth="22900" windowHeight="17560"/>
-    <workbookView minimized="1" xWindow="3520" yWindow="3320" windowWidth="25380" windowHeight="17560" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="12560" yWindow="0" windowWidth="12460" windowHeight="17260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="17560" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="T06_LockBox_Bom1" sheetId="1" r:id="rId1"/>
     <sheet name="Main_Board" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="184">
   <si>
     <t>Part</t>
   </si>
@@ -564,6 +564,15 @@
   </si>
   <si>
     <t>PCB - LCD</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main Board </t>
+  </si>
+  <si>
+    <t>LCD Board</t>
   </si>
 </sst>
 </file>
@@ -907,7 +916,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1102,8 +1111,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="242">
+  <cellStyleXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1346,35 +1418,24 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1409,17 +1470,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="242">
+  <cellStyles count="252">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1548,6 +1648,11 @@
     <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1653,6 +1758,11 @@
     <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1956,9 +2066,9 @@
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane xSplit="6900" activePane="topRight"/>
-      <selection activeCell="G42" sqref="G42"/>
-      <selection pane="topRight" activeCell="K42" sqref="K42"/>
+      <pane xSplit="8000" topLeftCell="J1"/>
+      <selection activeCell="B40" sqref="B40"/>
+      <selection pane="topRight" activeCell="M42" sqref="M42"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="D1" sqref="D1:D2"/>
@@ -1983,64 +2093,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="6"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="16"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="10">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="3">
         <v>1</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="3">
         <v>10</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="3">
         <v>100</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="4">
         <v>1000</v>
       </c>
     </row>
@@ -2072,16 +2182,16 @@
       <c r="I3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="23">
+      <c r="K3" s="14">
         <v>0.26</v>
       </c>
-      <c r="L3" s="23">
+      <c r="L3" s="14">
         <v>2.1800000000000002</v>
       </c>
-      <c r="M3" s="23">
+      <c r="M3" s="14">
         <v>10.88</v>
       </c>
-      <c r="N3" s="23">
+      <c r="N3" s="14">
         <v>63.92</v>
       </c>
     </row>
@@ -2113,16 +2223,16 @@
       <c r="I4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="23">
+      <c r="K4" s="14">
         <v>0.34</v>
       </c>
-      <c r="L4" s="23">
+      <c r="L4" s="14">
         <v>2.8</v>
       </c>
-      <c r="M4" s="23">
+      <c r="M4" s="14">
         <v>14</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="14">
         <v>82.25</v>
       </c>
     </row>
@@ -2154,16 +2264,16 @@
       <c r="I5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K5" s="23">
+      <c r="K5" s="14">
         <v>0.12</v>
       </c>
-      <c r="L5" s="23">
+      <c r="L5" s="14">
         <v>0.87</v>
       </c>
-      <c r="M5" s="23">
+      <c r="M5" s="14">
         <v>3.97</v>
       </c>
-      <c r="N5" s="23">
+      <c r="N5" s="14">
         <v>21.66</v>
       </c>
     </row>
@@ -2195,16 +2305,16 @@
       <c r="I6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K6" s="23">
+      <c r="K6" s="14">
         <v>0.32</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="14">
         <v>2.8</v>
       </c>
-      <c r="M6" s="23">
+      <c r="M6" s="14">
         <v>14</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="14">
         <v>92</v>
       </c>
     </row>
@@ -2236,16 +2346,16 @@
       <c r="I7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="14">
         <v>0.1</v>
       </c>
-      <c r="L7" s="23">
+      <c r="L7" s="14">
         <v>0.73</v>
       </c>
-      <c r="M7" s="23">
+      <c r="M7" s="14">
         <v>3.34</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="14">
         <v>18.21</v>
       </c>
     </row>
@@ -2277,16 +2387,16 @@
       <c r="I8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K8" s="23">
+      <c r="K8" s="14">
         <v>0.1</v>
       </c>
-      <c r="L8" s="23">
+      <c r="L8" s="14">
         <v>0.73</v>
       </c>
-      <c r="M8" s="23">
+      <c r="M8" s="14">
         <v>3.34</v>
       </c>
-      <c r="N8" s="23">
+      <c r="N8" s="14">
         <v>18.21</v>
       </c>
     </row>
@@ -2318,16 +2428,16 @@
       <c r="I9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="14">
         <v>0.1</v>
       </c>
-      <c r="L9" s="23">
+      <c r="L9" s="14">
         <v>0.73</v>
       </c>
-      <c r="M9" s="23">
+      <c r="M9" s="14">
         <v>3.34</v>
       </c>
-      <c r="N9" s="23">
+      <c r="N9" s="14">
         <v>18.21</v>
       </c>
     </row>
@@ -2359,16 +2469,16 @@
       <c r="I10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="14">
         <v>0.13</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="14">
         <v>1.2</v>
       </c>
-      <c r="M10" s="23">
+      <c r="M10" s="14">
         <v>7.88</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="14">
         <v>26.27</v>
       </c>
     </row>
@@ -2388,10 +2498,10 @@
       <c r="F11" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
@@ -2418,16 +2528,16 @@
       <c r="I12" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="14">
         <v>0.4</v>
       </c>
-      <c r="L12" s="23">
+      <c r="L12" s="14">
         <v>3.77</v>
       </c>
-      <c r="M12" s="23">
+      <c r="M12" s="14">
         <v>26.36</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="14">
         <v>188.3</v>
       </c>
     </row>
@@ -2456,16 +2566,16 @@
       <c r="I13" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="14">
         <v>0.32</v>
       </c>
-      <c r="L13" s="23">
+      <c r="L13" s="14">
         <v>3.07</v>
       </c>
-      <c r="M13" s="23">
+      <c r="M13" s="14">
         <v>21.51</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="14">
         <v>153.65</v>
       </c>
     </row>
@@ -2494,16 +2604,16 @@
       <c r="I14" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="14">
         <v>0.26</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="14">
         <v>2.48</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="14">
         <v>17.16</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="14">
         <v>118.8</v>
       </c>
     </row>
@@ -2535,16 +2645,16 @@
       <c r="I15" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K15" s="23" t="s">
+      <c r="K15" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="L15" s="23">
+      <c r="L15" s="14">
         <v>0.97</v>
       </c>
-      <c r="M15" s="23" t="s">
+      <c r="M15" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="14">
         <v>20.36</v>
       </c>
     </row>
@@ -2576,16 +2686,16 @@
       <c r="I16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="K16" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="L16" s="23">
+      <c r="L16" s="14">
         <v>0.97</v>
       </c>
-      <c r="M16" s="23" t="s">
+      <c r="M16" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="14">
         <v>20.36</v>
       </c>
     </row>
@@ -2617,16 +2727,16 @@
       <c r="I17" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K17" s="23" t="s">
+      <c r="K17" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="L17" s="23">
+      <c r="L17" s="14">
         <v>0.97</v>
       </c>
-      <c r="M17" s="23" t="s">
+      <c r="M17" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="N17" s="23">
+      <c r="N17" s="14">
         <v>20.36</v>
       </c>
     </row>
@@ -2658,16 +2768,16 @@
       <c r="I18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18" s="14">
         <v>0.1</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="M18" s="23">
+      <c r="M18" s="14">
         <v>2.19</v>
       </c>
-      <c r="N18" s="23">
+      <c r="N18" s="14">
         <v>8</v>
       </c>
     </row>
@@ -2699,16 +2809,16 @@
       <c r="I19" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="K19" s="23" t="s">
+      <c r="K19" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="L19" s="23">
+      <c r="L19" s="14">
         <v>0.97</v>
       </c>
-      <c r="M19" s="23" t="s">
+      <c r="M19" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="N19" s="23">
+      <c r="N19" s="14">
         <v>20.36</v>
       </c>
     </row>
@@ -2740,16 +2850,16 @@
       <c r="I20" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K20" s="23" t="s">
+      <c r="K20" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="L20" s="23">
+      <c r="L20" s="14">
         <v>0.97</v>
       </c>
-      <c r="M20" s="23" t="s">
+      <c r="M20" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="N20" s="23">
+      <c r="N20" s="14">
         <v>20.36</v>
       </c>
     </row>
@@ -2781,16 +2891,16 @@
       <c r="I21" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K21" s="23" t="s">
+      <c r="K21" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="L21" s="23">
+      <c r="L21" s="14">
         <v>0.97</v>
       </c>
-      <c r="M21" s="23" t="s">
+      <c r="M21" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="N21" s="23">
+      <c r="N21" s="14">
         <v>20.36</v>
       </c>
     </row>
@@ -2822,16 +2932,16 @@
       <c r="I22" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K22" s="23" t="s">
+      <c r="K22" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="L22" s="23">
+      <c r="L22" s="14">
         <v>0.97</v>
       </c>
-      <c r="M22" s="23" t="s">
+      <c r="M22" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="N22" s="23">
+      <c r="N22" s="14">
         <v>20.36</v>
       </c>
     </row>
@@ -2863,16 +2973,16 @@
       <c r="I23" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="K23" s="23">
+      <c r="K23" s="14">
         <v>0.1</v>
       </c>
-      <c r="L23" s="23" t="s">
+      <c r="L23" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="M23" s="23">
+      <c r="M23" s="14">
         <v>1.49</v>
       </c>
-      <c r="N23" s="23">
+      <c r="N23" s="14">
         <v>5.44</v>
       </c>
     </row>
@@ -2904,16 +3014,16 @@
       <c r="I24" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="K24" s="23">
+      <c r="K24" s="14">
         <v>0.1</v>
       </c>
-      <c r="L24" s="23" t="s">
+      <c r="L24" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="M24" s="23">
+      <c r="M24" s="14">
         <v>1.49</v>
       </c>
-      <c r="N24" s="23">
+      <c r="N24" s="14">
         <v>5.44</v>
       </c>
     </row>
@@ -2945,16 +3055,16 @@
       <c r="I25" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K25" s="23" t="s">
+      <c r="K25" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="L25" s="23">
+      <c r="L25" s="14">
         <v>0.97</v>
       </c>
-      <c r="M25" s="23" t="s">
+      <c r="M25" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="N25" s="23">
+      <c r="N25" s="14">
         <v>20.36</v>
       </c>
     </row>
@@ -2974,10 +3084,10 @@
       <c r="F26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
@@ -3004,16 +3114,16 @@
       <c r="I27" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K27" s="23">
+      <c r="K27" s="14">
         <v>0.19</v>
       </c>
-      <c r="L27" s="23">
+      <c r="L27" s="14">
         <v>1.73</v>
       </c>
-      <c r="M27" s="23">
+      <c r="M27" s="14">
         <v>11.34</v>
       </c>
-      <c r="N27" s="23">
+      <c r="N27" s="14">
         <v>37.799999999999997</v>
       </c>
     </row>
@@ -3042,16 +3152,16 @@
       <c r="I28" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K28" s="23">
+      <c r="K28" s="14">
         <v>0.19</v>
       </c>
-      <c r="L28" s="23">
+      <c r="L28" s="14">
         <v>1.73</v>
       </c>
-      <c r="M28" s="23">
+      <c r="M28" s="14">
         <v>11.34</v>
       </c>
-      <c r="N28" s="23">
+      <c r="N28" s="14">
         <v>37.799999999999997</v>
       </c>
     </row>
@@ -3080,16 +3190,16 @@
       <c r="I29" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K29" s="23">
+      <c r="K29" s="14">
         <v>0.19</v>
       </c>
-      <c r="L29" s="23">
+      <c r="L29" s="14">
         <v>1.73</v>
       </c>
-      <c r="M29" s="23">
+      <c r="M29" s="14">
         <v>11.34</v>
       </c>
-      <c r="N29" s="23">
+      <c r="N29" s="14">
         <v>37.799999999999997</v>
       </c>
     </row>
@@ -3118,16 +3228,16 @@
       <c r="I30" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="K30" s="23">
+      <c r="K30" s="14">
         <v>3.74</v>
       </c>
-      <c r="L30" s="23">
+      <c r="L30" s="14">
         <v>33.380000000000003</v>
       </c>
-      <c r="M30" s="23">
+      <c r="M30" s="14">
         <v>273.74</v>
       </c>
-      <c r="N30" s="23">
+      <c r="N30" s="14">
         <v>1869.45</v>
       </c>
     </row>
@@ -3156,16 +3266,16 @@
       <c r="I31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K31" s="23">
+      <c r="K31" s="14">
         <v>1.02</v>
       </c>
-      <c r="L31" s="23">
+      <c r="L31" s="14">
         <v>8.92</v>
       </c>
-      <c r="M31" s="23">
+      <c r="M31" s="14">
         <v>68.67</v>
       </c>
-      <c r="N31" s="23">
+      <c r="N31" s="14">
         <v>407.55</v>
       </c>
     </row>
@@ -3194,16 +3304,16 @@
       <c r="I32" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="K32" s="23">
+      <c r="K32" s="14">
         <v>1</v>
       </c>
-      <c r="L32" s="23">
+      <c r="L32" s="14">
         <v>7</v>
       </c>
-      <c r="M32" s="23">
+      <c r="M32" s="14">
         <v>47</v>
       </c>
-      <c r="N32" s="23">
+      <c r="N32" s="14">
         <v>340</v>
       </c>
     </row>
@@ -3232,16 +3342,16 @@
       <c r="I33" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="K33" s="23">
+      <c r="K33" s="14">
         <v>0.96</v>
       </c>
-      <c r="L33" s="23">
+      <c r="L33" s="14">
         <v>8.52</v>
       </c>
-      <c r="M33" s="23">
+      <c r="M33" s="14">
         <v>67.349999999999994</v>
       </c>
-      <c r="N33" s="23">
+      <c r="N33" s="14">
         <v>412.35</v>
       </c>
     </row>
@@ -3270,16 +3380,16 @@
       <c r="I34" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="K34" s="23">
+      <c r="K34" s="14">
         <v>0.56999999999999995</v>
       </c>
-      <c r="L34" s="23">
+      <c r="L34" s="14">
         <v>5.35</v>
       </c>
-      <c r="M34" s="23">
+      <c r="M34" s="14">
         <v>41.01</v>
       </c>
-      <c r="N34" s="23">
+      <c r="N34" s="14">
         <v>294.2</v>
       </c>
     </row>
@@ -3306,16 +3416,16 @@
         <v>125</v>
       </c>
       <c r="J35"/>
-      <c r="K35" s="23">
+      <c r="K35" s="14">
         <v>0.49</v>
       </c>
-      <c r="L35" s="23">
+      <c r="L35" s="14">
         <v>3.83</v>
       </c>
-      <c r="M35" s="23">
+      <c r="M35" s="14">
         <v>26.35</v>
       </c>
-      <c r="N35" s="23">
+      <c r="N35" s="14">
         <v>135.05000000000001</v>
       </c>
     </row>
@@ -3339,16 +3449,16 @@
         <v>154</v>
       </c>
       <c r="J36"/>
-      <c r="K36" s="23">
+      <c r="K36" s="14">
         <v>0.35</v>
       </c>
-      <c r="L36" s="23">
+      <c r="L36" s="14">
         <v>3.33</v>
       </c>
-      <c r="M36" s="23">
+      <c r="M36" s="14">
         <v>23.28</v>
       </c>
-      <c r="N36" s="23">
+      <c r="N36" s="14">
         <v>166.25</v>
       </c>
     </row>
@@ -3371,16 +3481,16 @@
       <c r="I37" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="K37" s="23">
+      <c r="K37" s="14">
         <v>0.43</v>
       </c>
-      <c r="L37" s="23">
+      <c r="L37" s="14">
         <v>3.99</v>
       </c>
-      <c r="M37" s="23">
+      <c r="M37" s="14">
         <v>30.59</v>
       </c>
-      <c r="N37" s="23">
+      <c r="N37" s="14">
         <v>219.45</v>
       </c>
     </row>
@@ -3397,16 +3507,16 @@
       <c r="J38" s="1">
         <v>1512</v>
       </c>
-      <c r="K38" s="23">
+      <c r="K38" s="14">
         <v>14.95</v>
       </c>
-      <c r="L38" s="23">
+      <c r="L38" s="14">
         <v>13.46</v>
       </c>
-      <c r="M38" s="23">
+      <c r="M38" s="14">
         <v>11.96</v>
       </c>
-      <c r="N38" s="23"/>
+      <c r="N38" s="14"/>
     </row>
     <row r="39" spans="1:14">
       <c r="B39" s="1" t="s">
@@ -3427,14 +3537,14 @@
       <c r="J39" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="K39" s="23">
+      <c r="K39" s="14">
         <v>7</v>
       </c>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
-      <c r="N39" s="23"/>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+    </row>
+    <row r="40" spans="1:14" ht="14" customHeight="1">
       <c r="B40" s="1" t="s">
         <v>28</v>
       </c>
@@ -3453,16 +3563,16 @@
       <c r="J40" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="K40" s="23">
+      <c r="K40" s="14">
         <v>12</v>
       </c>
-      <c r="L40" s="23">
+      <c r="L40" s="14">
         <v>105.6</v>
       </c>
-      <c r="M40" s="23">
+      <c r="M40" s="14">
         <v>948</v>
       </c>
-      <c r="N40" s="23">
+      <c r="N40" s="14">
         <f>2*4437.5</f>
         <v>8875</v>
       </c>
@@ -3542,341 +3652,450 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K24"/>
+  <dimension ref="B1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="H2" sqref="H2:K3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1"/>
-    <row r="2" spans="2:11">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="2:12" ht="15" thickBot="1">
+      <c r="B1" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
+      <c r="H1" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="31"/>
+    </row>
+    <row r="2" spans="2:12">
+      <c r="B2" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="22" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" ht="15" thickBot="1">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="22"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="22"/>
-    </row>
-    <row r="4" spans="2:11">
-      <c r="B4" s="15">
+      <c r="L2" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="15" thickBot="1">
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="25"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="25"/>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="16" t="str">
+      <c r="C4" s="9" t="str">
         <f>T06_LockBox_Bom1!B30</f>
         <v>ATMEGA328</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" spans="2:11">
-      <c r="B5" s="18">
+      <c r="E4" s="10"/>
+      <c r="F4" s="26">
+        <f>B4*T06_LockBox_Bom1!K30</f>
+        <v>3.74</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4">
+        <f>H4*T06_LockBox_Bom1!K40</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="13" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" s="18">
+      <c r="F5" s="27">
+        <f>B5*T06_LockBox_Bom1!K3</f>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="13" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="18">
+      <c r="F6" s="27">
+        <f>B6*T06_LockBox_Bom1!K4</f>
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="13" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="18">
+      <c r="F7" s="27">
+        <f>B7*T06_LockBox_Bom1!K5</f>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="11">
         <v>3</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="13" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="B9" s="18">
+      <c r="F8" s="27">
+        <f>B8*T06_LockBox_Bom1!K7</f>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="11">
         <v>1</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" s="18">
+      <c r="F9" s="27">
+        <f>T06_LockBox_Bom1!K36*B9/5</f>
+        <v>6.9999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="11">
         <v>1</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="2:11">
-      <c r="B11" s="18">
+      <c r="F10" s="27">
+        <f>B10*T06_LockBox_Bom1!K12</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="11">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="2:11">
-      <c r="B12" s="18">
+      <c r="F11" s="27">
+        <f>B11*T06_LockBox_Bom1!K13</f>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" s="11">
         <v>1</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="2:11">
-      <c r="B13" s="18">
+      <c r="F12" s="27">
+        <f>B12*T06_LockBox_Bom1!K14</f>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" s="11">
         <v>4</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="13" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="14" spans="2:11">
-      <c r="B14" s="18">
+      <c r="F13" s="27">
+        <f>B13*T06_LockBox_Bom1!L15/10</f>
+        <v>0.38800000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" s="11">
         <v>2</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="13" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="15" spans="2:11">
-      <c r="B15" s="18">
+      <c r="F14" s="27">
+        <f>B14*T06_LockBox_Bom1!K23</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="11">
         <v>1</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="13" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="16" spans="2:11">
-      <c r="B16" s="18">
+      <c r="F15" s="27">
+        <f>B15*T06_LockBox_Bom1!K18</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="11">
         <v>1</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="12">
         <v>150</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="13" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="18">
+      <c r="F16" s="27">
+        <f>B16*T06_LockBox_Bom1!L19/10</f>
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="11">
         <v>1</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="12">
         <v>33</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="13" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="18">
+      <c r="F17" s="27">
+        <f>B17*T06_LockBox_Bom1!L20/10</f>
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="11">
         <v>3</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="20"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="18">
+      <c r="E18" s="13"/>
+      <c r="F18" s="27">
+        <f>B18*T06_LockBox_Bom1!K27</f>
+        <v>0.57000000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="11">
         <v>1</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="20"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="18">
+      <c r="E19" s="13"/>
+      <c r="F19" s="27">
+        <f>B19*T06_LockBox_Bom1!K31</f>
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="11">
         <v>1</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="20"/>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="18">
+      <c r="E20" s="13"/>
+      <c r="F20" s="27">
+        <f>B20*T06_LockBox_Bom1!K32</f>
         <v>1</v>
       </c>
-      <c r="C21" s="19" t="s">
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="11">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E21" s="20"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="18">
+      <c r="E21" s="13"/>
+      <c r="F21" s="27">
+        <f>B21*T06_LockBox_Bom1!K33</f>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15" thickBot="1">
+      <c r="B22" s="5">
         <v>1</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="20"/>
-    </row>
-    <row r="23" spans="2:5" ht="15" thickBot="1">
-      <c r="B23" s="12">
-        <v>1</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="E23" s="14"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="28">
+        <f>T06_LockBox_Bom1!K34*B22</f>
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15" thickBot="1">
+      <c r="B23" s="5">
+        <f>SUM(B4:B22)</f>
+        <v>27</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="28">
+        <f>SUM(F4:F22)</f>
+        <v>10.812000000000001</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B1:F1"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
upadted the BOM; main, lcd and cable BOMS added
</commit_message>
<xml_diff>
--- a/eagle/T06_LockBox_bom.xlsx
+++ b/eagle/T06_LockBox_bom.xlsx
@@ -4,8 +4,8 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="0" windowWidth="12460" windowHeight="17260"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="17560" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="12000" yWindow="0" windowWidth="16720" windowHeight="17560"/>
+    <workbookView xWindow="1460" yWindow="280" windowWidth="25380" windowHeight="17560" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="T06_LockBox_Bom1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="210">
   <si>
     <t>Part</t>
   </si>
@@ -573,13 +573,92 @@
   </si>
   <si>
     <t>LCD Board</t>
+  </si>
+  <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>PCB to LCD Cable</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>MC10G-5-NG</t>
+  </si>
+  <si>
+    <t>3365/10 300SF</t>
+  </si>
+  <si>
+    <t>IDC Socket</t>
+  </si>
+  <si>
+    <t>Main to LCD ribbon cable connector - 10POS</t>
+  </si>
+  <si>
+    <t>Main to LCD ribbon cable - 10POS</t>
+  </si>
+  <si>
+    <t>1175-1435-ND</t>
+  </si>
+  <si>
+    <t>3030-10-0102-00</t>
+  </si>
+  <si>
+    <t>CNC TECH</t>
+  </si>
+  <si>
+    <t>j5</t>
+  </si>
+  <si>
+    <t>RJ45 Jack</t>
+  </si>
+  <si>
+    <t>RJ45 Keystone jack</t>
+  </si>
+  <si>
+    <t>PCH Cables</t>
+  </si>
+  <si>
+    <t>101703BE</t>
+  </si>
+  <si>
+    <t>1/4W</t>
+  </si>
+  <si>
+    <t>Nintendo Controller</t>
+  </si>
+  <si>
+    <t>ETHERNET CABLE</t>
+  </si>
+  <si>
+    <t>THE BOX</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>WOOD</t>
+  </si>
+  <si>
+    <t>HINGE</t>
+  </si>
+  <si>
+    <t>SCREWS</t>
+  </si>
+  <si>
+    <t>LATCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RJ45 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
@@ -916,7 +995,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1174,8 +1253,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="252">
+  <cellStyleXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1428,8 +1518,30 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1518,8 +1630,69 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="252">
+  <cellStyles count="274">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1653,6 +1826,17 @@
     <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1763,6 +1947,17 @@
     <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2063,12 +2258,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane xSplit="8000" topLeftCell="J1"/>
-      <selection activeCell="B40" sqref="B40"/>
-      <selection pane="topRight" activeCell="M42" sqref="M42"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane xSplit="8000" activePane="topRight"/>
+      <selection activeCell="K46" sqref="K46"/>
+      <selection pane="topRight" activeCell="B35" sqref="B35"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="D1" sqref="D1:D2"/>
@@ -3623,6 +3818,78 @@
       </c>
       <c r="N42" s="1" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K43" s="1">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="B44" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="L44" s="1">
+        <v>3.15</v>
+      </c>
+      <c r="M44" s="1">
+        <v>22.05</v>
+      </c>
+      <c r="N44" s="1">
+        <v>157.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="K45" s="1">
+        <v>2.0499999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -3652,19 +3919,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L23"/>
+  <dimension ref="B1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3744,13 +4012,15 @@
         <f>B4*T06_LockBox_Bom1!K30</f>
         <v>3.74</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="8">
         <v>1</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L4">
+      <c r="J4" s="9"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="41">
         <f>H4*T06_LockBox_Bom1!K40</f>
         <v>12</v>
       </c>
@@ -3772,6 +4042,20 @@
         <f>B5*T06_LockBox_Bom1!K3</f>
         <v>0.26</v>
       </c>
+      <c r="H5" s="11">
+        <v>1</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="42">
+        <f>H5*T06_LockBox_Bom1!K13</f>
+        <v>0.32</v>
+      </c>
     </row>
     <row r="6" spans="2:12">
       <c r="B6" s="11">
@@ -3790,6 +4074,22 @@
         <f>B6*T06_LockBox_Bom1!K4</f>
         <v>0.34</v>
       </c>
+      <c r="H6" s="11">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="L6" s="42">
+        <f>H6*T06_LockBox_Bom1!L15/10</f>
+        <v>9.7000000000000003E-2</v>
+      </c>
     </row>
     <row r="7" spans="2:12">
       <c r="B7" s="11">
@@ -3808,8 +4108,24 @@
         <f>B7*T06_LockBox_Bom1!K5</f>
         <v>0.12</v>
       </c>
-    </row>
-    <row r="8" spans="2:12">
+      <c r="H7" s="11">
+        <v>2</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="L7" s="42">
+        <f>H7*T06_LockBox_Bom1!K23</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="15" thickBot="1">
       <c r="B8" s="11">
         <v>3</v>
       </c>
@@ -3826,8 +4142,24 @@
         <f>B8*T06_LockBox_Bom1!K7</f>
         <v>0.30000000000000004</v>
       </c>
-    </row>
-    <row r="9" spans="2:12">
+      <c r="H8" s="5">
+        <v>2</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L8" s="43">
+        <f>H8*T06_LockBox_Bom1!K7</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickBot="1">
       <c r="B9" s="11">
         <v>1</v>
       </c>
@@ -3844,8 +4176,19 @@
         <f>T06_LockBox_Bom1!K36*B9/5</f>
         <v>6.9999999999999993E-2</v>
       </c>
-    </row>
-    <row r="10" spans="2:12">
+      <c r="H9" s="39">
+        <f>SUM(H4:H8)</f>
+        <v>7</v>
+      </c>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="44">
+        <f>SUM(L4:L8)</f>
+        <v>12.816999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15" thickBot="1">
       <c r="B10" s="11">
         <v>1</v>
       </c>
@@ -3863,7 +4206,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:12" ht="15" thickBot="1">
       <c r="B11" s="11">
         <v>1</v>
       </c>
@@ -3880,6 +4223,13 @@
         <f>B11*T06_LockBox_Bom1!K13</f>
         <v>0.32</v>
       </c>
+      <c r="H11" s="49" t="s">
+        <v>201</v>
+      </c>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="51"/>
     </row>
     <row r="12" spans="2:12">
       <c r="B12" s="11">
@@ -3898,8 +4248,23 @@
         <f>B12*T06_LockBox_Bom1!K14</f>
         <v>0.26</v>
       </c>
-    </row>
-    <row r="13" spans="2:12">
+      <c r="H12" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="15" thickBot="1">
       <c r="B13" s="11">
         <v>4</v>
       </c>
@@ -3916,6 +4281,11 @@
         <f>B13*T06_LockBox_Bom1!L15/10</f>
         <v>0.38800000000000001</v>
       </c>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="25"/>
     </row>
     <row r="14" spans="2:12">
       <c r="B14" s="11">
@@ -3934,6 +4304,18 @@
         <f>B14*T06_LockBox_Bom1!K23</f>
         <v>0.2</v>
       </c>
+      <c r="H14" s="8">
+        <v>1</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="45">
+        <f>H14*T06_LockBox_Bom1!K39</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="2:12">
       <c r="B15" s="11">
@@ -3952,8 +4334,19 @@
         <f>B15*T06_LockBox_Bom1!K18</f>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="16" spans="2:12">
+      <c r="H15" s="11">
+        <v>1</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="46">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="15" thickBot="1">
       <c r="B16" s="11">
         <v>1</v>
       </c>
@@ -3970,8 +4363,20 @@
         <f>B16*T06_LockBox_Bom1!L19/10</f>
         <v>9.7000000000000003E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:6">
+      <c r="H16" s="5">
+        <v>1</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="47">
+        <f>H16*T06_LockBox_Bom1!K34</f>
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="15" thickBot="1">
       <c r="B17" s="11">
         <v>1</v>
       </c>
@@ -3988,8 +4393,19 @@
         <f>B17*T06_LockBox_Bom1!L20/10</f>
         <v>9.7000000000000003E-2</v>
       </c>
-    </row>
-    <row r="18" spans="2:6">
+      <c r="H17" s="39">
+        <f>SUM(H14:H16)</f>
+        <v>3</v>
+      </c>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="48">
+        <f>SUM(L14:L16)</f>
+        <v>9.35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
       <c r="B18" s="11">
         <v>3</v>
       </c>
@@ -4005,7 +4421,7 @@
         <v>0.57000000000000006</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:12" ht="15" thickBot="1">
       <c r="B19" s="11">
         <v>1</v>
       </c>
@@ -4021,7 +4437,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:12" ht="15" thickBot="1">
       <c r="B20" s="11">
         <v>1</v>
       </c>
@@ -4036,8 +4452,15 @@
         <f>B20*T06_LockBox_Bom1!K32</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:6">
+      <c r="H20" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="31"/>
+    </row>
+    <row r="21" spans="2:12">
       <c r="B21" s="11">
         <v>1</v>
       </c>
@@ -4052,8 +4475,21 @@
         <f>B21*T06_LockBox_Bom1!K33</f>
         <v>0.96</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" ht="15" thickBot="1">
+      <c r="H21" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="K21" s="16"/>
+      <c r="L21" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="15" thickBot="1">
       <c r="B22" s="5">
         <v>1</v>
       </c>
@@ -4068,8 +4504,13 @@
         <f>T06_LockBox_Bom1!K34*B22</f>
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" ht="15" thickBot="1">
+      <c r="H22" s="20"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="25"/>
+    </row>
+    <row r="23" spans="2:12" ht="15" thickBot="1">
       <c r="B23" s="5">
         <f>SUM(B4:B22)</f>
         <v>27</v>
@@ -4081,11 +4522,123 @@
         <f>SUM(F4:F22)</f>
         <v>10.812000000000001</v>
       </c>
+      <c r="H23" s="8">
+        <v>1</v>
+      </c>
+      <c r="I23" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="J23" s="54"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="34"/>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="H24" s="11">
+        <v>1</v>
+      </c>
+      <c r="I24" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="J24" s="56"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="35"/>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="H25" s="11">
+        <v>1</v>
+      </c>
+      <c r="I25" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="J25" s="56"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="35"/>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="H26" s="11">
+        <v>1</v>
+      </c>
+      <c r="I26" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="J26" s="56"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="35"/>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="H27" s="11">
+        <v>1</v>
+      </c>
+      <c r="I27" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="J27" s="56"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="35"/>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="H28" s="11">
+        <v>1</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="J28" s="56"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="35"/>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="H29" s="11">
+        <v>1</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="J29" s="56"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="35"/>
+    </row>
+    <row r="30" spans="2:12" ht="15" thickBot="1">
+      <c r="H30" s="11">
+        <v>1</v>
+      </c>
+      <c r="I30" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="J30" s="56"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="35"/>
+    </row>
+    <row r="31" spans="2:12" ht="15" thickBot="1">
+      <c r="H31" s="36"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="31">
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="J21:K22"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="H1:L1"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="D2:D3"/>

</xml_diff>